<commit_message>
add workers to passwarde.xlsx
</commit_message>
<xml_diff>
--- a/final project/passwarde.xlsx
+++ b/final project/passwarde.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33AE69B-AC8B-477B-B5EF-30D2F9D4358F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D831CE-E3E3-45F8-9FA0-601745DBE2C7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t xml:space="preserve">user name </t>
   </si>
@@ -98,6 +98,33 @@
   </si>
   <si>
     <t>yoni@gmail.com</t>
+  </si>
+  <si>
+    <t>adir</t>
+  </si>
+  <si>
+    <t>rotem</t>
+  </si>
+  <si>
+    <t>stav</t>
+  </si>
+  <si>
+    <t>angel</t>
+  </si>
+  <si>
+    <t>drei</t>
+  </si>
+  <si>
+    <t>yaakobi</t>
+  </si>
+  <si>
+    <t>adir@gmail.com</t>
+  </si>
+  <si>
+    <t>rotem@gmail.com</t>
+  </si>
+  <si>
+    <t>stav@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -484,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -640,6 +667,69 @@
         <v>26</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8">
+        <v>123</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8">
+        <v>111111114</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9">
+        <v>123</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9">
+        <v>111111115</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10">
+        <v>123</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10">
+        <v>111111116</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="1"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{C356BEF1-26AF-4C70-A608-8E455D9E44B9}"/>
@@ -648,9 +738,12 @@
     <hyperlink ref="F5" r:id="rId4" xr:uid="{C5BE7160-EFBD-46DE-9F71-6442294B31AC}"/>
     <hyperlink ref="F6" r:id="rId5" xr:uid="{3F510F8F-0863-4876-B8F5-2212BCD05DAF}"/>
     <hyperlink ref="F7" r:id="rId6" xr:uid="{64EA1464-557D-4FDF-A968-B2027EF66627}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{DCEE048E-3FE8-40BF-81C9-444A06D7887C}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{0E57AFF3-F746-490A-91B4-A1CDF04564DD}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{65F21430-8BCA-4970-9F7E-91689FD8A89D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>